<commit_message>
more tweaks to spreadsheet
</commit_message>
<xml_diff>
--- a/investigate recoveries.xlsx
+++ b/investigate recoveries.xlsx
@@ -690,6 +690,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -710,6 +711,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -726,12 +728,19 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -760,7 +769,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -771,6 +780,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -790,10 +807,11 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <font>
         <name val="Lohit Devanagari"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF333333"/>
       </font>
@@ -810,6 +828,21 @@
         <diagonal/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF996600"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -824,7 +857,7 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -882,7 +915,7 @@
   <dimension ref="A1:G213"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -890,9 +923,9 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.16"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
@@ -2193,27 +2226,27 @@
         <v>0.276249312845213</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="3" t="n">
         <v>93</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C53" s="0" t="n">
+      <c r="C53" s="3" t="n">
         <v>1193078</v>
       </c>
-      <c r="D53" s="0" t="n">
+      <c r="D53" s="3" t="n">
         <v>753050</v>
       </c>
-      <c r="E53" s="0" t="n">
+      <c r="E53" s="3" t="n">
         <v>549947</v>
       </c>
-      <c r="F53" s="1" t="n">
+      <c r="F53" s="4" t="n">
         <f aca="false">(D53-E53)/D53</f>
         <v>0.269707190757586</v>
       </c>
-      <c r="G53" s="1" t="n">
+      <c r="G53" s="4" t="n">
         <f aca="false">ABS(F53)</f>
         <v>0.269707190757586</v>
       </c>
@@ -6222,6 +6255,11 @@
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>1000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" priority="3" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6498,7 +6536,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="0" t="str">
@@ -6901,7 +6939,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B51" s="0" t="str">
@@ -7228,7 +7266,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>